<commit_message>
Updated file through July 6
</commit_message>
<xml_diff>
--- a/Agenda-items/HCA stats.xlsx
+++ b/Agenda-items/HCA stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="25360" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,16 +207,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="42">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -225,6 +233,10 @@
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -241,6 +253,10 @@
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -577,7 +593,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -593,44 +609,46 @@
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="E1" s="6">
+      <c r="C1" s="9"/>
+      <c r="E1" s="8">
         <v>42551</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="6">
+      <c r="H1" s="9"/>
+      <c r="I1" s="8">
         <v>42556</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8">
+        <v>42557</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
     </row>
     <row r="2" spans="1:32" s="1" customFormat="1">
       <c r="B2" s="2" t="s">
@@ -730,8 +748,8 @@
         <v>7</v>
       </c>
       <c r="B3" s="4">
-        <f>SUM(E3,G3,I3)</f>
-        <v>272</v>
+        <f t="array" ref="B3">SUM(IF($E3:$XFD3&gt;1,$E3:$XFD3,0))</f>
+        <v>514</v>
       </c>
       <c r="E3" s="4">
         <f>SUM(E5:E12)</f>
@@ -747,7 +765,7 @@
       </c>
       <c r="K3" s="4">
         <f>SUM(K5:K12)</f>
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="M3" s="4">
         <f>SUM(M5:M12)</f>
@@ -795,106 +813,106 @@
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <f>SUM(E5,G5,I5)</f>
-        <v>8</v>
+        <f t="array" ref="B5">SUM(IF($E5:$XFD5&gt;1,$E5:$XFD5,0))</f>
+        <v>18</v>
       </c>
       <c r="C5" s="5">
-        <f>B5/B$3</f>
-        <v>2.9411764705882353E-2</v>
+        <f t="shared" ref="C5:C12" si="0">B5/B$3</f>
+        <v>3.5019455252918288E-2</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>4</v>
       </c>
       <c r="F5" s="5">
         <f>E5/E$3</f>
         <v>3.9215686274509803E-2</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>2</v>
       </c>
       <c r="H5" s="5">
         <f>G5/G$3</f>
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>2</v>
       </c>
       <c r="J5" s="5">
         <f>I5/I$3</f>
         <v>2.4390243902439025E-2</v>
       </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5" t="str">
+      <c r="K5" s="7">
+        <v>10</v>
+      </c>
+      <c r="L5" s="5">
         <f>IF(K5=0,"",K5/K$3)</f>
-        <v/>
-      </c>
-      <c r="M5" s="9">
+        <v>4.1322314049586778E-2</v>
+      </c>
+      <c r="M5" s="7">
         <v>0</v>
       </c>
       <c r="N5" s="5" t="str">
         <f>IF(M5=0,"",M5/M$3)</f>
         <v/>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="7">
         <v>0</v>
       </c>
       <c r="P5" s="5" t="str">
         <f>IF(O5=0,"",O5/O$3)</f>
         <v/>
       </c>
-      <c r="Q5" s="9">
+      <c r="Q5" s="7">
         <v>0</v>
       </c>
       <c r="R5" s="5" t="str">
         <f>IF(Q5=0,"",Q5/Q$3)</f>
         <v/>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="7">
         <v>0</v>
       </c>
       <c r="T5" s="5" t="str">
         <f>IF(S5=0,"",S5/S$3)</f>
         <v/>
       </c>
-      <c r="U5" s="9">
+      <c r="U5" s="7">
         <v>0</v>
       </c>
       <c r="V5" s="5" t="str">
         <f>IF(U5=0,"",U5/U$3)</f>
         <v/>
       </c>
-      <c r="W5" s="9">
+      <c r="W5" s="7">
         <v>0</v>
       </c>
       <c r="X5" s="5" t="str">
         <f>IF(W5=0,"",W5/W$3)</f>
         <v/>
       </c>
-      <c r="Y5" s="9">
+      <c r="Y5" s="7">
         <v>0</v>
       </c>
       <c r="Z5" s="5" t="str">
         <f>IF(Y5=0,"",Y5/Y$3)</f>
         <v/>
       </c>
-      <c r="AA5" s="9">
+      <c r="AA5" s="7">
         <v>0</v>
       </c>
       <c r="AB5" s="5" t="str">
         <f>IF(AA5=0,"",AA5/AA$3)</f>
         <v/>
       </c>
-      <c r="AC5" s="9">
+      <c r="AC5" s="7">
         <v>0</v>
       </c>
       <c r="AD5" s="5" t="str">
         <f>IF(AC5=0,"",AC5/AC$3)</f>
         <v/>
       </c>
-      <c r="AE5" s="9">
+      <c r="AE5" s="7">
         <v>0</v>
       </c>
       <c r="AF5" s="5" t="str">
@@ -907,110 +925,110 @@
         <v>2</v>
       </c>
       <c r="B6" s="4">
-        <f>SUM(E6,G6,I6)</f>
-        <v>10</v>
+        <f t="array" ref="B6">SUM(IF($E6:$XFD6&gt;1,$E6:$XFD6,0))</f>
+        <v>15</v>
       </c>
       <c r="C6" s="5">
-        <f>B6/B$3</f>
-        <v>3.6764705882352942E-2</v>
+        <f t="shared" si="0"/>
+        <v>2.9182879377431907E-2</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>5</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" ref="F6:H12" si="0">E6/E$3</f>
+        <f t="shared" ref="F6:F12" si="1">E6/E$3</f>
         <v>4.9019607843137254E-2</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>3</v>
       </c>
       <c r="H6" s="5">
-        <f t="shared" si="0"/>
+        <f>G6/G$3</f>
         <v>3.4090909090909088E-2</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>2</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" ref="J6:L6" si="1">I6/I$3</f>
+        <f t="shared" ref="J6" si="2">I6/I$3</f>
         <v>2.4390243902439025E-2</v>
       </c>
-      <c r="K6" s="9">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5" t="str">
-        <f t="shared" ref="L6:N12" si="2">IF(K6=0,"",K6/K$3)</f>
-        <v/>
-      </c>
-      <c r="M6" s="9">
+      <c r="K6" s="7">
+        <v>5</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ref="L6:N12" si="3">IF(K6=0,"",K6/K$3)</f>
+        <v>2.0661157024793389E-2</v>
+      </c>
+      <c r="M6" s="7">
         <v>0</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O6" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O6" s="7">
         <v>0</v>
       </c>
       <c r="P6" s="5" t="str">
-        <f t="shared" ref="P6" si="3">IF(O6=0,"",O6/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q6" s="9">
+        <f t="shared" ref="P6" si="4">IF(O6=0,"",O6/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q6" s="7">
         <v>0</v>
       </c>
       <c r="R6" s="5" t="str">
-        <f t="shared" ref="R6" si="4">IF(Q6=0,"",Q6/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S6" s="9">
+        <f t="shared" ref="R6" si="5">IF(Q6=0,"",Q6/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S6" s="7">
         <v>0</v>
       </c>
       <c r="T6" s="5" t="str">
-        <f t="shared" ref="T6" si="5">IF(S6=0,"",S6/S$3)</f>
-        <v/>
-      </c>
-      <c r="U6" s="9">
+        <f t="shared" ref="T6" si="6">IF(S6=0,"",S6/S$3)</f>
+        <v/>
+      </c>
+      <c r="U6" s="7">
         <v>0</v>
       </c>
       <c r="V6" s="5" t="str">
-        <f t="shared" ref="V6" si="6">IF(U6=0,"",U6/U$3)</f>
-        <v/>
-      </c>
-      <c r="W6" s="9">
+        <f t="shared" ref="V6" si="7">IF(U6=0,"",U6/U$3)</f>
+        <v/>
+      </c>
+      <c r="W6" s="7">
         <v>0</v>
       </c>
       <c r="X6" s="5" t="str">
-        <f t="shared" ref="X6" si="7">IF(W6=0,"",W6/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y6" s="9">
+        <f t="shared" ref="X6" si="8">IF(W6=0,"",W6/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y6" s="7">
         <v>0</v>
       </c>
       <c r="Z6" s="5" t="str">
-        <f t="shared" ref="Z6" si="8">IF(Y6=0,"",Y6/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA6" s="9">
+        <f t="shared" ref="Z6" si="9">IF(Y6=0,"",Y6/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA6" s="7">
         <v>0</v>
       </c>
       <c r="AB6" s="5" t="str">
-        <f t="shared" ref="AB6" si="9">IF(AA6=0,"",AA6/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC6" s="9">
+        <f t="shared" ref="AB6" si="10">IF(AA6=0,"",AA6/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC6" s="7">
         <v>0</v>
       </c>
       <c r="AD6" s="5" t="str">
-        <f t="shared" ref="AD6" si="10">IF(AC6=0,"",AC6/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE6" s="9">
+        <f t="shared" ref="AD6" si="11">IF(AC6=0,"",AC6/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE6" s="7">
         <v>0</v>
       </c>
       <c r="AF6" s="5" t="str">
-        <f t="shared" ref="AF6" si="11">IF(AE6=0,"",AE6/AE$3)</f>
+        <f t="shared" ref="AF6" si="12">IF(AE6=0,"",AE6/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1019,110 +1037,110 @@
         <v>3</v>
       </c>
       <c r="B7" s="4">
-        <f>SUM(E7,G7,I7)</f>
-        <v>27</v>
+        <f t="array" ref="B7">SUM(IF($E7:$XFD7&gt;1,$E7:$XFD7,0))</f>
+        <v>53</v>
       </c>
       <c r="C7" s="5">
-        <f>B7/B$3</f>
-        <v>9.9264705882352935E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.10311284046692606</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>6</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>11</v>
       </c>
       <c r="H7" s="5">
-        <f t="shared" si="0"/>
+        <f>G7/G$3</f>
         <v>0.125</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>10</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" ref="J7:L7" si="12">I7/I$3</f>
+        <f t="shared" ref="J7" si="13">I7/I$3</f>
         <v>0.12195121951219512</v>
       </c>
-      <c r="K7" s="9">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M7" s="9">
+      <c r="K7" s="7">
+        <v>26</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" si="3"/>
+        <v>0.10743801652892562</v>
+      </c>
+      <c r="M7" s="7">
         <v>0</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O7" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O7" s="7">
         <v>0</v>
       </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" ref="P7" si="13">IF(O7=0,"",O7/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q7" s="9">
+        <f t="shared" ref="P7" si="14">IF(O7=0,"",O7/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q7" s="7">
         <v>0</v>
       </c>
       <c r="R7" s="5" t="str">
-        <f t="shared" ref="R7" si="14">IF(Q7=0,"",Q7/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S7" s="9">
+        <f t="shared" ref="R7" si="15">IF(Q7=0,"",Q7/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S7" s="7">
         <v>0</v>
       </c>
       <c r="T7" s="5" t="str">
-        <f t="shared" ref="T7" si="15">IF(S7=0,"",S7/S$3)</f>
-        <v/>
-      </c>
-      <c r="U7" s="9">
+        <f t="shared" ref="T7" si="16">IF(S7=0,"",S7/S$3)</f>
+        <v/>
+      </c>
+      <c r="U7" s="7">
         <v>0</v>
       </c>
       <c r="V7" s="5" t="str">
-        <f t="shared" ref="V7" si="16">IF(U7=0,"",U7/U$3)</f>
-        <v/>
-      </c>
-      <c r="W7" s="9">
+        <f t="shared" ref="V7" si="17">IF(U7=0,"",U7/U$3)</f>
+        <v/>
+      </c>
+      <c r="W7" s="7">
         <v>0</v>
       </c>
       <c r="X7" s="5" t="str">
-        <f t="shared" ref="X7" si="17">IF(W7=0,"",W7/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y7" s="9">
+        <f t="shared" ref="X7" si="18">IF(W7=0,"",W7/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y7" s="7">
         <v>0</v>
       </c>
       <c r="Z7" s="5" t="str">
-        <f t="shared" ref="Z7" si="18">IF(Y7=0,"",Y7/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA7" s="9">
+        <f t="shared" ref="Z7" si="19">IF(Y7=0,"",Y7/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA7" s="7">
         <v>0</v>
       </c>
       <c r="AB7" s="5" t="str">
-        <f t="shared" ref="AB7" si="19">IF(AA7=0,"",AA7/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC7" s="9">
+        <f t="shared" ref="AB7" si="20">IF(AA7=0,"",AA7/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC7" s="7">
         <v>0</v>
       </c>
       <c r="AD7" s="5" t="str">
-        <f t="shared" ref="AD7" si="20">IF(AC7=0,"",AC7/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE7" s="9">
+        <f t="shared" ref="AD7" si="21">IF(AC7=0,"",AC7/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE7" s="7">
         <v>0</v>
       </c>
       <c r="AF7" s="5" t="str">
-        <f t="shared" ref="AF7" si="21">IF(AE7=0,"",AE7/AE$3)</f>
+        <f t="shared" ref="AF7" si="22">IF(AE7=0,"",AE7/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1131,110 +1149,110 @@
         <v>10</v>
       </c>
       <c r="B8" s="4">
-        <f>SUM(E8,G8,I8)</f>
+        <f t="array" ref="B8">SUM(IF($E8:$XFD8&gt;1,$E8:$XFD8,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
-        <f>B8/B$3</f>
-        <v>3.6764705882352941E-3</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
       <c r="F8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.8039215686274508E-3</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>0</v>
       </c>
       <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
+        <f>G8/G$3</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
         <v>0</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" ref="J8:L8" si="22">I8/I$3</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M8" s="9">
+        <f t="shared" ref="J8:L8" si="23">I8/I$3</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
         <v>0</v>
       </c>
       <c r="N8" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O8" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O8" s="7">
         <v>0</v>
       </c>
       <c r="P8" s="5" t="str">
-        <f t="shared" ref="P8" si="23">IF(O8=0,"",O8/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q8" s="9">
+        <f t="shared" ref="P8" si="24">IF(O8=0,"",O8/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q8" s="7">
         <v>0</v>
       </c>
       <c r="R8" s="5" t="str">
-        <f t="shared" ref="R8" si="24">IF(Q8=0,"",Q8/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S8" s="9">
+        <f t="shared" ref="R8" si="25">IF(Q8=0,"",Q8/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S8" s="7">
         <v>0</v>
       </c>
       <c r="T8" s="5" t="str">
-        <f t="shared" ref="T8" si="25">IF(S8=0,"",S8/S$3)</f>
-        <v/>
-      </c>
-      <c r="U8" s="9">
+        <f t="shared" ref="T8" si="26">IF(S8=0,"",S8/S$3)</f>
+        <v/>
+      </c>
+      <c r="U8" s="7">
         <v>0</v>
       </c>
       <c r="V8" s="5" t="str">
-        <f t="shared" ref="V8" si="26">IF(U8=0,"",U8/U$3)</f>
-        <v/>
-      </c>
-      <c r="W8" s="9">
+        <f t="shared" ref="V8" si="27">IF(U8=0,"",U8/U$3)</f>
+        <v/>
+      </c>
+      <c r="W8" s="7">
         <v>0</v>
       </c>
       <c r="X8" s="5" t="str">
-        <f t="shared" ref="X8" si="27">IF(W8=0,"",W8/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y8" s="9">
+        <f t="shared" ref="X8" si="28">IF(W8=0,"",W8/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y8" s="7">
         <v>0</v>
       </c>
       <c r="Z8" s="5" t="str">
-        <f t="shared" ref="Z8" si="28">IF(Y8=0,"",Y8/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA8" s="9">
+        <f t="shared" ref="Z8" si="29">IF(Y8=0,"",Y8/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA8" s="7">
         <v>0</v>
       </c>
       <c r="AB8" s="5" t="str">
-        <f t="shared" ref="AB8" si="29">IF(AA8=0,"",AA8/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC8" s="9">
+        <f t="shared" ref="AB8" si="30">IF(AA8=0,"",AA8/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC8" s="7">
         <v>0</v>
       </c>
       <c r="AD8" s="5" t="str">
-        <f t="shared" ref="AD8" si="30">IF(AC8=0,"",AC8/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE8" s="9">
+        <f t="shared" ref="AD8" si="31">IF(AC8=0,"",AC8/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE8" s="7">
         <v>0</v>
       </c>
       <c r="AF8" s="5" t="str">
-        <f t="shared" ref="AF8" si="31">IF(AE8=0,"",AE8/AE$3)</f>
+        <f t="shared" ref="AF8" si="32">IF(AE8=0,"",AE8/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1243,110 +1261,110 @@
         <v>4</v>
       </c>
       <c r="B9" s="4">
-        <f>SUM(E9,G9,I9)</f>
+        <f t="array" ref="B9">SUM(IF($E9:$XFD9&gt;1,$E9:$XFD9,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
-        <f>B9/B$3</f>
-        <v>3.6764705882352941E-3</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
       <c r="H9" s="5">
-        <f t="shared" si="0"/>
+        <f>G9/G$3</f>
         <v>1.1363636363636364E-2</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>0</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" ref="J9:L9" si="32">I9/I$3</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M9" s="9">
+        <f t="shared" ref="J9:L9" si="33">I9/I$3</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
         <v>0</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O9" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O9" s="7">
         <v>0</v>
       </c>
       <c r="P9" s="5" t="str">
-        <f t="shared" ref="P9" si="33">IF(O9=0,"",O9/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q9" s="9">
+        <f t="shared" ref="P9" si="34">IF(O9=0,"",O9/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q9" s="7">
         <v>0</v>
       </c>
       <c r="R9" s="5" t="str">
-        <f t="shared" ref="R9" si="34">IF(Q9=0,"",Q9/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S9" s="9">
+        <f t="shared" ref="R9" si="35">IF(Q9=0,"",Q9/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S9" s="7">
         <v>0</v>
       </c>
       <c r="T9" s="5" t="str">
-        <f t="shared" ref="T9" si="35">IF(S9=0,"",S9/S$3)</f>
-        <v/>
-      </c>
-      <c r="U9" s="9">
+        <f t="shared" ref="T9" si="36">IF(S9=0,"",S9/S$3)</f>
+        <v/>
+      </c>
+      <c r="U9" s="7">
         <v>0</v>
       </c>
       <c r="V9" s="5" t="str">
-        <f t="shared" ref="V9" si="36">IF(U9=0,"",U9/U$3)</f>
-        <v/>
-      </c>
-      <c r="W9" s="9">
+        <f t="shared" ref="V9" si="37">IF(U9=0,"",U9/U$3)</f>
+        <v/>
+      </c>
+      <c r="W9" s="7">
         <v>0</v>
       </c>
       <c r="X9" s="5" t="str">
-        <f t="shared" ref="X9" si="37">IF(W9=0,"",W9/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y9" s="9">
+        <f t="shared" ref="X9" si="38">IF(W9=0,"",W9/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y9" s="7">
         <v>0</v>
       </c>
       <c r="Z9" s="5" t="str">
-        <f t="shared" ref="Z9" si="38">IF(Y9=0,"",Y9/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA9" s="9">
+        <f t="shared" ref="Z9" si="39">IF(Y9=0,"",Y9/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA9" s="7">
         <v>0</v>
       </c>
       <c r="AB9" s="5" t="str">
-        <f t="shared" ref="AB9" si="39">IF(AA9=0,"",AA9/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC9" s="9">
+        <f t="shared" ref="AB9" si="40">IF(AA9=0,"",AA9/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC9" s="7">
         <v>0</v>
       </c>
       <c r="AD9" s="5" t="str">
-        <f t="shared" ref="AD9" si="40">IF(AC9=0,"",AC9/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE9" s="9">
+        <f t="shared" ref="AD9" si="41">IF(AC9=0,"",AC9/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE9" s="7">
         <v>0</v>
       </c>
       <c r="AF9" s="5" t="str">
-        <f t="shared" ref="AF9" si="41">IF(AE9=0,"",AE9/AE$3)</f>
+        <f t="shared" ref="AF9" si="42">IF(AE9=0,"",AE9/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1355,110 +1373,110 @@
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <f>SUM(E10,G10,I10)</f>
-        <v>24</v>
+        <f t="array" ref="B10">SUM(IF($E10:$XFD10&gt;1,$E10:$XFD10,0))</f>
+        <v>41</v>
       </c>
       <c r="C10" s="5">
-        <f>B10/B$3</f>
-        <v>8.8235294117647065E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.9766536964980539E-2</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>11</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.10784313725490197</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>6</v>
       </c>
       <c r="H10" s="5">
-        <f t="shared" si="0"/>
+        <f>G10/G$3</f>
         <v>6.8181818181818177E-2</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>7</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" ref="J10:L10" si="42">I10/I$3</f>
+        <f t="shared" ref="J10" si="43">I10/I$3</f>
         <v>8.5365853658536592E-2</v>
       </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M10" s="9">
+      <c r="K10" s="7">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" si="3"/>
+        <v>7.0247933884297523E-2</v>
+      </c>
+      <c r="M10" s="7">
         <v>0</v>
       </c>
       <c r="N10" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O10" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O10" s="7">
         <v>0</v>
       </c>
       <c r="P10" s="5" t="str">
-        <f t="shared" ref="P10" si="43">IF(O10=0,"",O10/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q10" s="9">
+        <f t="shared" ref="P10" si="44">IF(O10=0,"",O10/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q10" s="7">
         <v>0</v>
       </c>
       <c r="R10" s="5" t="str">
-        <f t="shared" ref="R10" si="44">IF(Q10=0,"",Q10/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S10" s="9">
+        <f t="shared" ref="R10" si="45">IF(Q10=0,"",Q10/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S10" s="7">
         <v>0</v>
       </c>
       <c r="T10" s="5" t="str">
-        <f t="shared" ref="T10" si="45">IF(S10=0,"",S10/S$3)</f>
-        <v/>
-      </c>
-      <c r="U10" s="9">
+        <f t="shared" ref="T10" si="46">IF(S10=0,"",S10/S$3)</f>
+        <v/>
+      </c>
+      <c r="U10" s="7">
         <v>0</v>
       </c>
       <c r="V10" s="5" t="str">
-        <f t="shared" ref="V10" si="46">IF(U10=0,"",U10/U$3)</f>
-        <v/>
-      </c>
-      <c r="W10" s="9">
+        <f t="shared" ref="V10" si="47">IF(U10=0,"",U10/U$3)</f>
+        <v/>
+      </c>
+      <c r="W10" s="7">
         <v>0</v>
       </c>
       <c r="X10" s="5" t="str">
-        <f t="shared" ref="X10" si="47">IF(W10=0,"",W10/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y10" s="9">
+        <f t="shared" ref="X10" si="48">IF(W10=0,"",W10/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y10" s="7">
         <v>0</v>
       </c>
       <c r="Z10" s="5" t="str">
-        <f t="shared" ref="Z10" si="48">IF(Y10=0,"",Y10/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA10" s="9">
+        <f t="shared" ref="Z10" si="49">IF(Y10=0,"",Y10/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA10" s="7">
         <v>0</v>
       </c>
       <c r="AB10" s="5" t="str">
-        <f t="shared" ref="AB10" si="49">IF(AA10=0,"",AA10/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC10" s="9">
+        <f t="shared" ref="AB10" si="50">IF(AA10=0,"",AA10/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC10" s="7">
         <v>0</v>
       </c>
       <c r="AD10" s="5" t="str">
-        <f t="shared" ref="AD10" si="50">IF(AC10=0,"",AC10/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE10" s="9">
+        <f t="shared" ref="AD10" si="51">IF(AC10=0,"",AC10/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE10" s="7">
         <v>0</v>
       </c>
       <c r="AF10" s="5" t="str">
-        <f t="shared" ref="AF10" si="51">IF(AE10=0,"",AE10/AE$3)</f>
+        <f t="shared" ref="AF10" si="52">IF(AE10=0,"",AE10/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1467,110 +1485,110 @@
         <v>0</v>
       </c>
       <c r="B11" s="4">
-        <f>SUM(E11,G11,I11)</f>
-        <v>121</v>
+        <f t="array" ref="B11">SUM(IF($E11:$XFD11&gt;1,$E11:$XFD11,0))</f>
+        <v>211</v>
       </c>
       <c r="C11" s="5">
-        <f>B11/B$3</f>
-        <v>0.44485294117647056</v>
+        <f t="shared" si="0"/>
+        <v>0.41050583657587547</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>46</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.45098039215686275</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>38</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" si="0"/>
+        <f>G11/G$3</f>
         <v>0.43181818181818182</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>37</v>
       </c>
       <c r="J11" s="5">
-        <f t="shared" ref="J11:L11" si="52">I11/I$3</f>
+        <f t="shared" ref="J11" si="53">I11/I$3</f>
         <v>0.45121951219512196</v>
       </c>
-      <c r="K11" s="9">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M11" s="9">
+      <c r="K11" s="7">
+        <v>90</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="3"/>
+        <v>0.37190082644628097</v>
+      </c>
+      <c r="M11" s="7">
         <v>0</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O11" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O11" s="7">
         <v>0</v>
       </c>
       <c r="P11" s="5" t="str">
-        <f t="shared" ref="P11" si="53">IF(O11=0,"",O11/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q11" s="9">
+        <f t="shared" ref="P11" si="54">IF(O11=0,"",O11/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q11" s="7">
         <v>0</v>
       </c>
       <c r="R11" s="5" t="str">
-        <f t="shared" ref="R11" si="54">IF(Q11=0,"",Q11/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S11" s="9">
+        <f t="shared" ref="R11" si="55">IF(Q11=0,"",Q11/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S11" s="7">
         <v>0</v>
       </c>
       <c r="T11" s="5" t="str">
-        <f t="shared" ref="T11" si="55">IF(S11=0,"",S11/S$3)</f>
-        <v/>
-      </c>
-      <c r="U11" s="9">
+        <f t="shared" ref="T11" si="56">IF(S11=0,"",S11/S$3)</f>
+        <v/>
+      </c>
+      <c r="U11" s="7">
         <v>0</v>
       </c>
       <c r="V11" s="5" t="str">
-        <f t="shared" ref="V11" si="56">IF(U11=0,"",U11/U$3)</f>
-        <v/>
-      </c>
-      <c r="W11" s="9">
+        <f t="shared" ref="V11" si="57">IF(U11=0,"",U11/U$3)</f>
+        <v/>
+      </c>
+      <c r="W11" s="7">
         <v>0</v>
       </c>
       <c r="X11" s="5" t="str">
-        <f t="shared" ref="X11" si="57">IF(W11=0,"",W11/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y11" s="9">
+        <f t="shared" ref="X11" si="58">IF(W11=0,"",W11/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y11" s="7">
         <v>0</v>
       </c>
       <c r="Z11" s="5" t="str">
-        <f t="shared" ref="Z11" si="58">IF(Y11=0,"",Y11/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA11" s="9">
+        <f t="shared" ref="Z11" si="59">IF(Y11=0,"",Y11/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA11" s="7">
         <v>0</v>
       </c>
       <c r="AB11" s="5" t="str">
-        <f t="shared" ref="AB11" si="59">IF(AA11=0,"",AA11/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC11" s="9">
+        <f t="shared" ref="AB11" si="60">IF(AA11=0,"",AA11/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC11" s="7">
         <v>0</v>
       </c>
       <c r="AD11" s="5" t="str">
-        <f t="shared" ref="AD11" si="60">IF(AC11=0,"",AC11/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE11" s="9">
+        <f t="shared" ref="AD11" si="61">IF(AC11=0,"",AC11/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE11" s="7">
         <v>0</v>
       </c>
       <c r="AF11" s="5" t="str">
-        <f t="shared" ref="AF11" si="61">IF(AE11=0,"",AE11/AE$3)</f>
+        <f t="shared" ref="AF11" si="62">IF(AE11=0,"",AE11/AE$3)</f>
         <v/>
       </c>
     </row>
@@ -1579,138 +1597,138 @@
         <v>6</v>
       </c>
       <c r="B12" s="4">
-        <f>SUM(E12,G12,I12)</f>
-        <v>80</v>
+        <f t="array" ref="B12">SUM(IF($E12:$XFD12&gt;1,$E12:$XFD12,0))</f>
+        <v>174</v>
       </c>
       <c r="C12" s="5">
-        <f>B12/B$3</f>
-        <v>0.29411764705882354</v>
+        <f t="shared" si="0"/>
+        <v>0.33852140077821014</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>29</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.28431372549019607</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>27</v>
       </c>
       <c r="H12" s="5">
-        <f t="shared" si="0"/>
+        <f>G12/G$3</f>
         <v>0.30681818181818182</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>24</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" ref="J12:L12" si="62">I12/I$3</f>
+        <f t="shared" ref="J12" si="63">I12/I$3</f>
         <v>0.29268292682926828</v>
       </c>
-      <c r="K12" s="9">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M12" s="9">
+      <c r="K12" s="7">
+        <v>94</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" si="3"/>
+        <v>0.38842975206611569</v>
+      </c>
+      <c r="M12" s="7">
         <v>0</v>
       </c>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="O12" s="9">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="O12" s="7">
         <v>0</v>
       </c>
       <c r="P12" s="5" t="str">
-        <f t="shared" ref="P12" si="63">IF(O12=0,"",O12/O$3)</f>
-        <v/>
-      </c>
-      <c r="Q12" s="9">
+        <f t="shared" ref="P12" si="64">IF(O12=0,"",O12/O$3)</f>
+        <v/>
+      </c>
+      <c r="Q12" s="7">
         <v>0</v>
       </c>
       <c r="R12" s="5" t="str">
-        <f t="shared" ref="R12" si="64">IF(Q12=0,"",Q12/Q$3)</f>
-        <v/>
-      </c>
-      <c r="S12" s="9">
+        <f t="shared" ref="R12" si="65">IF(Q12=0,"",Q12/Q$3)</f>
+        <v/>
+      </c>
+      <c r="S12" s="7">
         <v>0</v>
       </c>
       <c r="T12" s="5" t="str">
-        <f t="shared" ref="T12" si="65">IF(S12=0,"",S12/S$3)</f>
-        <v/>
-      </c>
-      <c r="U12" s="9">
+        <f t="shared" ref="T12" si="66">IF(S12=0,"",S12/S$3)</f>
+        <v/>
+      </c>
+      <c r="U12" s="7">
         <v>0</v>
       </c>
       <c r="V12" s="5" t="str">
-        <f t="shared" ref="V12" si="66">IF(U12=0,"",U12/U$3)</f>
-        <v/>
-      </c>
-      <c r="W12" s="9">
+        <f t="shared" ref="V12" si="67">IF(U12=0,"",U12/U$3)</f>
+        <v/>
+      </c>
+      <c r="W12" s="7">
         <v>0</v>
       </c>
       <c r="X12" s="5" t="str">
-        <f t="shared" ref="X12" si="67">IF(W12=0,"",W12/W$3)</f>
-        <v/>
-      </c>
-      <c r="Y12" s="9">
+        <f t="shared" ref="X12" si="68">IF(W12=0,"",W12/W$3)</f>
+        <v/>
+      </c>
+      <c r="Y12" s="7">
         <v>0</v>
       </c>
       <c r="Z12" s="5" t="str">
-        <f t="shared" ref="Z12" si="68">IF(Y12=0,"",Y12/Y$3)</f>
-        <v/>
-      </c>
-      <c r="AA12" s="9">
+        <f t="shared" ref="Z12" si="69">IF(Y12=0,"",Y12/Y$3)</f>
+        <v/>
+      </c>
+      <c r="AA12" s="7">
         <v>0</v>
       </c>
       <c r="AB12" s="5" t="str">
-        <f t="shared" ref="AB12" si="69">IF(AA12=0,"",AA12/AA$3)</f>
-        <v/>
-      </c>
-      <c r="AC12" s="9">
+        <f t="shared" ref="AB12" si="70">IF(AA12=0,"",AA12/AA$3)</f>
+        <v/>
+      </c>
+      <c r="AC12" s="7">
         <v>0</v>
       </c>
       <c r="AD12" s="5" t="str">
-        <f t="shared" ref="AD12" si="70">IF(AC12=0,"",AC12/AC$3)</f>
-        <v/>
-      </c>
-      <c r="AE12" s="9">
+        <f t="shared" ref="AD12" si="71">IF(AC12=0,"",AC12/AC$3)</f>
+        <v/>
+      </c>
+      <c r="AE12" s="7">
         <v>0</v>
       </c>
       <c r="AF12" s="5" t="str">
-        <f t="shared" ref="AF12" si="71">IF(AE12=0,"",AE12/AE$3)</f>
+        <f t="shared" ref="AF12" si="72">IF(AE12=0,"",AE12/AE$3)</f>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:32">
-      <c r="J13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Z13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AF13" s="8"/>
+      <c r="J13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AB13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AF13" s="6"/>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="4">
-        <f>SUM(B5+B6+B7+B8+B9+B12)</f>
-        <v>127</v>
+        <f t="array" ref="B14">SUM(IF($E14:$XFD14&gt;1,$E14:$XFD14,0))</f>
+        <v>262</v>
       </c>
       <c r="C14" s="5">
         <f>IF(B14=0,"",B14/B3)</f>
-        <v>0.46691176470588236</v>
+        <v>0.50972762645914393</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4">
@@ -1739,11 +1757,11 @@
       </c>
       <c r="K14" s="4">
         <f>SUM(K5+K6+K7+K8+K9+K12)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="5" t="str">
+        <v>135</v>
+      </c>
+      <c r="L14" s="5">
         <f>IF(K14=0,"",K14/K3)</f>
-        <v/>
+        <v>0.55785123966942152</v>
       </c>
       <c r="M14" s="4">
         <f>SUM(M5+M6+M7+M8+M9+M12)</f>
@@ -1837,12 +1855,12 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>